<commit_message>
update conspect update stats
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF56B7A-2851-4436-9D8E-600B02E5E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A6040A-B04C-42F2-9274-5B2B08F0E28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
@@ -332,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -407,6 +407,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,10 +622,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.55813953488372092</c:v>
+                  <c:v>0.58139534883720934</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9215686274509803E-2</c:v>
+                  <c:v>6.741573033707865E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -6448,7 +6451,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6488,7 +6491,7 @@
       </c>
       <c r="B2" s="13">
         <f>Java!A3*100%/Java!B3</f>
-        <v>0.55813953488372092</v>
+        <v>0.58139534883720934</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>30</v>
@@ -6505,15 +6508,16 @@
       </c>
       <c r="B3" s="13">
         <f>Java!A6*100%/Java!B6</f>
-        <v>3.9215686274509803E-2</v>
+        <v>6.741573033707865E-2</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="21">
         <f ca="1">SUM(B2:B19)/D1</f>
-        <v>4.0626894261954337E-2</v>
-      </c>
+        <v>4.4057284796358162E-2</v>
+      </c>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="str">
@@ -6529,7 +6533,7 @@
       </c>
       <c r="D4" s="22">
         <f ca="1">13/D3</f>
-        <v>319.98507973999983</v>
+        <v>295.07038529697587</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6538,7 +6542,7 @@
       </c>
       <c r="D5" s="20">
         <f ca="1">DATE(2022,7,17) + D4</f>
-        <v>45078.985079739999</v>
+        <v>45054.070385296975</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6643,6 +6647,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -6652,7 +6657,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6682,7 +6687,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="6">
         <v>43</v>
@@ -6704,10 +6709,10 @@
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6">
-        <v>153</v>
+        <v>12</v>
+      </c>
+      <c r="B6" s="29">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update stats update questions
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A6040A-B04C-42F2-9274-5B2B08F0E28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189CD8CE-8531-4946-A94A-FB5F24BB02A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
@@ -390,6 +390,9 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -407,9 +410,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,7 +625,7 @@
                   <c:v>0.58139534883720934</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.741573033707865E-2</c:v>
+                  <c:v>6.7039106145251395E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -6508,14 +6508,14 @@
       </c>
       <c r="B3" s="13">
         <f>Java!A6*100%/Java!B6</f>
-        <v>6.741573033707865E-2</v>
+        <v>6.7039106145251395E-2</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="21">
         <f ca="1">SUM(B2:B19)/D1</f>
-        <v>4.4057284796358162E-2</v>
+        <v>4.4032176516903013E-2</v>
       </c>
       <c r="E3" s="21"/>
     </row>
@@ -6533,7 +6533,7 @@
       </c>
       <c r="D4" s="22">
         <f ca="1">13/D3</f>
-        <v>295.07038529697587</v>
+        <v>295.2386420191965</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="D5" s="20">
         <f ca="1">DATE(2022,7,17) + D4</f>
-        <v>45054.070385296975</v>
+        <v>45054.238642019198</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6657,7 +6657,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6672,10 +6672,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6694,10 +6694,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="27"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -6711,15 +6711,15 @@
       <c r="A6" s="5">
         <v>12</v>
       </c>
-      <c r="B6" s="29">
-        <v>178</v>
+      <c r="B6" s="23">
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="27"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -6764,10 +6764,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6786,10 +6786,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="25"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -6808,10 +6808,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="25"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -6855,10 +6855,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6877,10 +6877,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="25"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -6899,10 +6899,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="26"/>
+      <c r="B7" s="27"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -6946,10 +6946,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6990,10 +6990,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="25"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -7035,10 +7035,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -7060,10 +7060,10 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="25"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">

</xml_diff>

<commit_message>
update semaphore update conspect update progress
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9627F21A-5486-4096-9203-9C96D6B70945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0C0167-6C3A-4983-8F88-531066669334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
@@ -622,10 +622,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.58139534883720934</c:v>
+                  <c:v>0.62790697674418605</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.7039106145251395E-2</c:v>
+                  <c:v>7.2625698324022353E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -6474,7 +6474,7 @@
       </c>
       <c r="D1" s="19">
         <f ca="1">TODAY() - DATE(2022,7,17)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>29</v>
@@ -6491,14 +6491,14 @@
       </c>
       <c r="B2" s="13">
         <f>Java!A3*100%/Java!B3</f>
-        <v>0.58139534883720934</v>
+        <v>0.62790697674418605</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="19">
         <f ca="1">F1-TODAY()</f>
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -6508,14 +6508,14 @@
       </c>
       <c r="B3" s="13">
         <f>Java!A6*100%/Java!B6</f>
-        <v>6.7039106145251395E-2</v>
+        <v>7.2625698324022353E-2</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="21">
         <f ca="1">SUM(B2:B19)/D1</f>
-        <v>4.4032176516903013E-2</v>
+        <v>4.4536304239955797E-2</v>
       </c>
       <c r="E3" s="21"/>
     </row>
@@ -6533,7 +6533,7 @@
       </c>
       <c r="D4" s="22">
         <f ca="1">13/D3</f>
-        <v>295.2386420191965</v>
+        <v>291.89669465965778</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="D5" s="20">
         <f ca="1">DATE(2022,7,17) + D4</f>
-        <v>45054.238642019198</v>
+        <v>45050.896694659656</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6657,7 +6657,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6687,7 +6687,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6">
         <v>43</v>
@@ -6709,7 +6709,7 @@
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="23">
         <v>179</v>

</xml_diff>

<commit_message>
update questions update progress
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0C0167-6C3A-4983-8F88-531066669334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20744FE-8081-464A-9ED0-5CB369EC8959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -625,7 +625,7 @@
                   <c:v>0.62790697674418605</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.2625698324022353E-2</c:v>
+                  <c:v>7.8212290502793297E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -5935,13 +5935,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>973862</xdr:colOff>
+      <xdr:colOff>973863</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>79460</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>849924</xdr:colOff>
+      <xdr:colOff>190501</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>165945</xdr:rowOff>
     </xdr:to>
@@ -5977,7 +5977,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>871904</xdr:colOff>
+      <xdr:colOff>210695</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>108060</xdr:rowOff>
     </xdr:to>
@@ -6007,15 +6007,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>923888</xdr:colOff>
+      <xdr:colOff>253855</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>94770</xdr:rowOff>
+      <xdr:rowOff>81632</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>564174</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>360395</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>181255</xdr:rowOff>
+      <xdr:rowOff>168117</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6043,15 +6043,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>934877</xdr:colOff>
+      <xdr:colOff>264843</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>17183</xdr:rowOff>
+      <xdr:rowOff>4045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>51616</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>446690</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>102907</xdr:rowOff>
+      <xdr:rowOff>89769</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6085,7 +6085,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>857251</xdr:colOff>
+      <xdr:colOff>196113</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>42117</xdr:rowOff>
     </xdr:to>
@@ -6115,15 +6115,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>909966</xdr:colOff>
+      <xdr:colOff>239932</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>168115</xdr:rowOff>
+      <xdr:rowOff>154977</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>26705</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>421779</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>56770</xdr:rowOff>
+      <xdr:rowOff>43632</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6450,8 +6450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6508,14 +6508,14 @@
       </c>
       <c r="B3" s="13">
         <f>Java!A6*100%/Java!B6</f>
-        <v>7.2625698324022353E-2</v>
+        <v>7.8212290502793297E-2</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="21">
         <f ca="1">SUM(B2:B19)/D1</f>
-        <v>4.4536304239955797E-2</v>
+        <v>4.4885466251128985E-2</v>
       </c>
       <c r="E3" s="21"/>
     </row>
@@ -6533,7 +6533,7 @@
       </c>
       <c r="D4" s="22">
         <f ca="1">13/D3</f>
-        <v>291.89669465965778</v>
+        <v>289.62604347845036</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="D5" s="20">
         <f ca="1">DATE(2022,7,17) + D4</f>
-        <v>45050.896694659656</v>
+        <v>45048.626043478449</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6656,8 +6656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D29483B-5B77-4D6C-8B76-A9E21F260E99}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6709,7 +6709,7 @@
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="23">
         <v>179</v>

</xml_diff>

<commit_message>
update deadlock example add test for deadlock example update progress
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20744FE-8081-464A-9ED0-5CB369EC8959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B6EBC0-6A6A-449E-B4F1-CB7594A995D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
@@ -622,7 +622,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.62790697674418605</c:v>
+                  <c:v>0.65116279069767447</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7.8212290502793297E-2</c:v>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="B2" s="13">
         <f>Java!A3*100%/Java!B3</f>
-        <v>0.62790697674418605</v>
+        <v>0.65116279069767447</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>30</v>
@@ -6515,7 +6515,7 @@
       </c>
       <c r="D3" s="21">
         <f ca="1">SUM(B2:B19)/D1</f>
-        <v>4.4885466251128985E-2</v>
+        <v>4.633895462322201E-2</v>
       </c>
       <c r="E3" s="21"/>
     </row>
@@ -6533,7 +6533,7 @@
       </c>
       <c r="D4" s="22">
         <f ca="1">13/D3</f>
-        <v>289.62604347845036</v>
+        <v>280.54150348668554</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="D5" s="20">
         <f ca="1">DATE(2022,7,17) + D4</f>
-        <v>45048.626043478449</v>
+        <v>45039.541503486689</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6657,7 +6657,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6687,7 +6687,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="6">
         <v>43</v>

</xml_diff>

<commit_message>
update DB conspect, update interwiew questions
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4091AD08-AD64-43B3-BEFE-E11077300212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FABD3E5-468C-4EED-9D43-357AF10CF180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -1393,7 +1393,7 @@
                   <c:v>6.8965517241379309E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.9411764705882353E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -6450,8 +6450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6459,7 +6459,7 @@
     <col min="1" max="1" width="46.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="16" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="14" style="18" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" style="17" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
@@ -6496,7 +6496,7 @@
       <c r="C2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="20">
+      <c r="D2" s="19">
         <f ca="1">$F$1-TODAY()</f>
         <v>14</v>
       </c>
@@ -6515,7 +6515,7 @@
       </c>
       <c r="D3" s="21">
         <f ca="1">SUM($B$2:$B$100)/$D$1</f>
-        <v>4.770962397319517E-2</v>
+        <v>4.9439727779423549E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6532,7 +6532,7 @@
       </c>
       <c r="D4" s="22">
         <f ca="1">13/$D$3</f>
-        <v>272.4817115998195</v>
+        <v>262.94643162275872</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6541,7 +6541,7 @@
       </c>
       <c r="D5" s="20">
         <f ca="1">DATE(2022,7,17) + $D$4</f>
-        <v>45031.481711599823</v>
+        <v>45021.94643162276</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6591,7 +6591,7 @@
       </c>
       <c r="B11" s="16">
         <f>'Базы данных'!A6*100%/'Базы данных'!B6</f>
-        <v>0</v>
+        <v>2.9411764705882353E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -6655,8 +6655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D29483B-5B77-4D6C-8B76-A9E21F260E99}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6843,7 +6843,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6891,10 +6891,10 @@
     </row>
     <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="8">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update progress and DB conspect
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FABD3E5-468C-4EED-9D43-357AF10CF180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85127C96-ECC4-43B0-9F54-12C35CAC98F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="1530" yWindow="2595" windowWidth="28320" windowHeight="15345" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Лекций просмотрено</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>Дней с начала обучения прошло:</t>
+  </si>
+  <si>
+    <t>Spring в действии (Книга)</t>
+  </si>
+  <si>
+    <t>Прочитано</t>
+  </si>
+  <si>
+    <t>Дейт. Введение в системы баз данных (книга)</t>
   </si>
 </sst>
 </file>
@@ -1283,9 +1292,9 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Анализ!$A$10:$A$12</c:f>
+              <c:f>Анализ!$A$10:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>PostgreSql (курс)</c:v>
                 </c:pt>
@@ -1294,6 +1303,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Задачки SQL (LeetCode)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Дейт. Введение в системы баз данных (книга)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1368,9 +1380,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Анализ!$A$10:$A$12</c:f>
+              <c:f>Анализ!$A$10:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>PostgreSql (курс)</c:v>
                 </c:pt>
@@ -1380,22 +1392,28 @@
                 <c:pt idx="2">
                   <c:v>Задачки SQL (LeetCode)</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>Дейт. Введение в системы баз данных (книга)</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Анализ!$B$10:$B$12</c:f>
+              <c:f>Анализ!$B$10:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.8965517241379309E-3</c:v>
+                  <c:v>1.3793103448275862E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.9411764705882353E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1662,7 +1680,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Анализ!$A$14</c:f>
+              <c:f>Анализ!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1741,7 +1759,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Анализ!$A$14</c:f>
+              <c:f>Анализ!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1752,7 +1770,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Анализ!$B$14</c:f>
+              <c:f>Анализ!$B$15</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -2024,7 +2042,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Анализ!$A$16</c:f>
+              <c:f>Анализ!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2103,7 +2121,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Анализ!$A$16</c:f>
+              <c:f>Анализ!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2114,7 +2132,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Анализ!$B$16</c:f>
+              <c:f>Анализ!$B$17</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -2386,14 +2404,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Анализ!$A$18:$A$19</c:f>
+              <c:f>Анализ!$A$19:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Spring (курс)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Spring проекты (курс)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spring в действии (Книга)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2468,28 +2489,34 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Анализ!$A$18:$A$19</c:f>
+              <c:f>Анализ!$A$19:$A$21</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Spring (курс)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Spring проекты (курс)</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>Spring в действии (Книга)</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Анализ!$B$18:$B$19</c:f>
+              <c:f>Анализ!$B$19:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6448,15 +6475,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="52.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" style="16" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="18" customWidth="1"/>
@@ -6515,7 +6542,7 @@
       </c>
       <c r="D3" s="21">
         <f ca="1">SUM($B$2:$B$100)/$D$1</f>
-        <v>4.9439727779423549E-2</v>
+        <v>4.9845407292608133E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -6531,8 +6558,8 @@
         <v>27</v>
       </c>
       <c r="D4" s="22">
-        <f ca="1">13/$D$3</f>
-        <v>262.94643162275872</v>
+        <f ca="1">COUNTA(B2:B100)/$D$3</f>
+        <v>300.93043300750475</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -6541,7 +6568,7 @@
       </c>
       <c r="D5" s="20">
         <f ca="1">DATE(2022,7,17) + $D$4</f>
-        <v>45021.94643162276</v>
+        <v>45059.930433007503</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -6581,7 +6608,7 @@
       </c>
       <c r="B10" s="16">
         <f>'Базы данных'!A3*100%/'Базы данных'!B3</f>
-        <v>6.8965517241379309E-3</v>
+        <v>1.3793103448275862E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -6604,43 +6631,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="str">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="str">
+        <f>'Базы данных'!A10</f>
+        <v>Дейт. Введение в системы баз данных (книга)</v>
+      </c>
+      <c r="B13" s="16">
+        <f>'Базы данных'!A12*100%/'Базы данных'!B12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="str">
         <f>Сети!A1</f>
         <v>Введение в комп. сети (Андрей)</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B15" s="16">
         <f>Сети!A3*100%/Сети!B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="str">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="str">
         <f>Git!A1</f>
         <v>Git (курс)</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B17" s="16">
         <f>Git!A3*100%/Git!B3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="str">
-        <f>Spring!A1</f>
-        <v>Spring (курс)</v>
-      </c>
-      <c r="B18" s="16">
-        <f>Spring!A3*100%/Spring!B3</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="str">
+        <f>Spring!A1</f>
+        <v>Spring (курс)</v>
+      </c>
+      <c r="B19" s="16">
+        <f>Spring!A3*100%/Spring!B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="str">
         <f>Spring!A4</f>
         <v>Spring проекты (курс)</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B20" s="16">
         <f>Spring!A6*100%/Spring!B6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="str">
+        <f>Spring!A7</f>
+        <v>Spring в действии (Книга)</v>
+      </c>
+      <c r="B21" s="16">
+        <f>Spring!A9*100%/Spring!B9</f>
         <v>0</v>
       </c>
     </row>
@@ -6752,7 +6799,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6825,7 +6872,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="6">
-        <v>288</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -6840,16 +6887,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846B637B-365E-45A8-ACB1-45E326A5872F}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -6869,7 +6916,7 @@
     </row>
     <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="8">
         <v>145</v>
@@ -6912,18 +6959,41 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="7">
         <v>0</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="8">
         <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="25"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>0</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1076</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7020,10 +7090,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCB3B14-49A5-43EF-AB59-F62EEDF89BCA}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7073,18 +7143,42 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="7">
         <v>0</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="8">
         <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6">
+        <v>468</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update conspect DB update questions update progress
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85127C96-ECC4-43B0-9F54-12C35CAC98F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7778625-0BA3-4270-A4D2-AEA0C6EF4025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="2595" windowWidth="28320" windowHeight="15345" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="6075" yWindow="1860" windowWidth="28320" windowHeight="15345" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>Лекций просмотрено</t>
   </si>
@@ -146,6 +146,21 @@
   <si>
     <t>Дейт. Введение в системы баз данных (книга)</t>
   </si>
+  <si>
+    <t>[41;1117]</t>
+  </si>
+  <si>
+    <t>[18;273]</t>
+  </si>
+  <si>
+    <t>Spring вопросы на собеседовании</t>
+  </si>
+  <si>
+    <t>[23; 954]</t>
+  </si>
+  <si>
+    <t>Компьютерные сети (книга)</t>
+  </si>
 </sst>
 </file>
 
@@ -154,7 +169,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,13 +193,57 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -341,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -372,15 +431,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -420,6 +475,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -428,7 +497,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF3399FF"/>
+      <color rgb="FF99FF99"/>
+      <color rgb="FFCCECFF"/>
+      <color rgb="FFFFCCFF"/>
       <color rgb="FFE785D2"/>
+      <color rgb="FFC438F6"/>
     </mruColors>
   </colors>
   <extLst>
@@ -541,7 +615,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="E785D2"/>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -551,14 +627,16 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="0">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -579,7 +657,7 @@
                 <a:endParaRPr lang="ru-RU"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -589,21 +667,16 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -845,10 +918,7 @@
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -877,10 +947,7 @@
           <a:pPr>
             <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -940,25 +1007,25 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1082,10 +1149,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1142,10 +1206,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -1198,7 +1259,11 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="ru-RU"/>
     </a:p>
@@ -1312,7 +1377,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1414,7 +1482,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>9.2936802973977699E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1680,11 +1748,14 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Анализ!$A$15</c:f>
+              <c:f>Анализ!$A$15:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Введение в комп. сети (Андрей)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Компьютерные сети (книга)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1759,22 +1830,28 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Анализ!$A$15</c:f>
+              <c:f>Анализ!$A$15:$A$16</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>Введение в комп. сети (Андрей)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Компьютерные сети (книга)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Анализ!$B$15</c:f>
+              <c:f>Анализ!$B$15:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2042,7 +2119,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Анализ!$A$17</c:f>
+              <c:f>Анализ!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2121,7 +2198,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Анализ!$A$17</c:f>
+              <c:f>Анализ!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2132,7 +2209,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Анализ!$B$17</c:f>
+              <c:f>Анализ!$B$18</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -2404,7 +2481,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Анализ!$A$19:$A$21</c:f>
+              <c:f>Анализ!$A$20:$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2489,7 +2566,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Анализ!$A$19:$A$21</c:f>
+              <c:f>Анализ!$A$20:$A$22</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2506,7 +2583,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Анализ!$B$19:$B$21</c:f>
+              <c:f>Анализ!$B$20:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -6175,6 +6252,131 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>115957</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>162616</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3129575" cy="1183657"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45FA5AE8-1920-94B1-39DA-B0472D67ECA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="115957" y="4734616"/>
+          <a:ext cx="3129575" cy="1183657"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1400" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>!ПРИМЕЧАНИЕ!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Выполнение абсолютно всех пунктов не обязательно.</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Поэтому анализ является сильно примерным, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>но он явно отражет весь прогресс обучения.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Так же нужно учитывать, что я самостоятельно,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>по мере изучения, добавляю вопросы, которые могут</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>быть на собеседованиях.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6475,219 +6677,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="14" customWidth="1"/>
     <col min="3" max="3" width="41.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="18" customWidth="1"/>
+    <col min="4" max="4" width="14" style="16" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="15" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="28" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="19">
+      <c r="D1" s="17">
         <f ca="1">TODAY() - DATE(2022,7,17)</f>
         <v>17</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="20">
+      <c r="F1" s="18">
         <f>DATE(2022,8,17)</f>
         <v>44790</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="str">
+      <c r="A2" s="29" t="str">
         <f>Java!A1</f>
         <v>Продвинутая Java (курс)</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <f>Java!A3*100%/Java!B3</f>
         <v>0.69767441860465118</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="17">
         <f ca="1">$F$1-TODAY()</f>
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="str">
+      <c r="A3" s="30" t="str">
         <f>Java!A4</f>
         <v>Java вопросы собеседований</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <f>Java!A6*100%/Java!B6</f>
         <v>9.4444444444444442E-2</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="19">
         <f ca="1">SUM($B$2:$B$100)/$D$1</f>
-        <v>4.9845407292608133E-2</v>
+        <v>5.0392094368925645E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="str">
+      <c r="A4" s="30" t="str">
         <f>Java!A7</f>
         <v>Практика Java (курс)</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <f>Java!A9*100%/Java!B9</f>
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="20">
         <f ca="1">COUNTA(B2:B100)/$D$3</f>
-        <v>300.93043300750475</v>
+        <v>337.35450397320801</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="18">
         <f ca="1">DATE(2022,7,17) + $D$4</f>
-        <v>45059.930433007503</v>
+        <v>45096.354503973205</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="str">
+      <c r="A6" s="35" t="str">
         <f>АиСД!A1</f>
         <v>Задачи для собеседований Java LeetCode</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="14">
         <f>АиСД!A3*100%/АиСД!B3</f>
         <v>1.2048192771084338E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="str">
+      <c r="A7" s="35" t="str">
         <f>АиСД!A4</f>
         <v>Алгоритмы и структуры данных (Алишев)</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <f>АиСД!A6*100%/АиСД!B6</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="str">
+      <c r="A8" s="35" t="str">
         <f>АиСД!A7</f>
         <v>Книга Грокаем Алгоритмы</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="14">
         <f>АиСД!A9*100%/АиСД!B9</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="str">
+      <c r="A10" s="39" t="str">
         <f>'Базы данных'!A1</f>
         <v>PostgreSql (курс)</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="14">
         <f>'Базы данных'!A3*100%/'Базы данных'!B3</f>
         <v>1.3793103448275862E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="str">
+      <c r="A11" s="39" t="str">
         <f>'Базы данных'!A4</f>
         <v>Вопросы SQL</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="14">
         <f>'Базы данных'!A6*100%/'Базы данных'!B6</f>
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="str">
+      <c r="A12" s="39" t="str">
         <f>'Базы данных'!A7</f>
         <v>Задачки SQL (LeetCode)</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="14">
         <f>'Базы данных'!A9*100%/'Базы данных'!B9</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="str">
+      <c r="A13" s="39" t="str">
         <f>'Базы данных'!A10</f>
         <v>Дейт. Введение в системы баз данных (книга)</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="14">
         <f>'Базы данных'!A12*100%/'Базы данных'!B12</f>
-        <v>0</v>
+        <v>9.2936802973977699E-3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="str">
+      <c r="A15" s="36" t="str">
         <f>Сети!A1</f>
         <v>Введение в комп. сети (Андрей)</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="14">
         <f>Сети!A3*100%/Сети!B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="str">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="str">
+        <f>Сети!A4</f>
+        <v>Компьютерные сети (книга)</v>
+      </c>
+      <c r="B16" s="14">
+        <f>Сети!A6*100%/Сети!B6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="str">
         <f>Git!A1</f>
         <v>Git (курс)</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B18" s="14">
         <f>Git!A3*100%/Git!B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="str">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="38" t="str">
         <f>Spring!A1</f>
         <v>Spring (курс)</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B20" s="14">
         <f>Spring!A3*100%/Spring!B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="str">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="str">
         <f>Spring!A4</f>
         <v>Spring проекты (курс)</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B21" s="14">
         <f>Spring!A6*100%/Spring!B6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="str">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="str">
         <f>Spring!A7</f>
         <v>Spring в действии (Книга)</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B22" s="14">
         <f>Spring!A9*100%/Spring!B9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="38" t="str">
+        <f>Spring!A10</f>
+        <v>Spring вопросы на собеседовании</v>
+      </c>
+      <c r="B23" s="14">
+        <f>Spring!A12*100%/Spring!B12</f>
         <v>0</v>
       </c>
     </row>
@@ -6718,10 +6940,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="23"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -6740,10 +6962,10 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="25"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -6757,15 +6979,15 @@
       <c r="A6" s="5">
         <v>17</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="21">
         <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="25"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -6796,10 +7018,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CEB77C-D1D9-44FA-A033-AAFB087AD5F9}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6809,13 +7031,13 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="23"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -6823,7 +7045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -6831,13 +7053,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="23"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -6845,7 +7067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>0</v>
       </c>
@@ -6853,13 +7075,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -6867,12 +7089,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>0</v>
       </c>
       <c r="B9" s="6">
         <v>255</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -6887,10 +7112,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846B637B-365E-45A8-ACB1-45E326A5872F}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6900,13 +7125,13 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="23"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -6914,7 +7139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -6922,13 +7147,13 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="23"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -6936,7 +7161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -6944,13 +7169,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="25"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -6958,7 +7183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>0</v>
       </c>
@@ -6966,13 +7191,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="23"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>33</v>
       </c>
@@ -6980,12 +7205,16 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>0</v>
+        <f>51-41</f>
+        <v>10</v>
       </c>
       <c r="B12" s="6">
         <v>1076</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -7001,10 +7230,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFCCA27-2B5A-43A0-8328-6BD008C1B7A2}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7014,13 +7243,13 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="23"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -7028,17 +7257,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="8">
         <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="23"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6">
+        <v>931</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7059,10 +7314,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="23"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -7090,10 +7345,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCB3B14-49A5-43EF-AB59-F62EEDF89BCA}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7104,10 +7359,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="29"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -7129,10 +7384,10 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="23"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -7151,10 +7406,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="25"/>
+      <c r="B7" s="23"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -7165,18 +7420,41 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="7">
         <v>0</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="8">
         <v>468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="23"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="33">
+        <v>0</v>
+      </c>
+      <c r="B12" s="34">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
update conspect and progress
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FEA18E-34FC-4F5A-8D8D-F1F2E37F7182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DBD8DD-CEF3-43B5-8F4E-7442108E2EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="2520" windowWidth="35670" windowHeight="18330" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="1200" yWindow="2325" windowWidth="35670" windowHeight="18330" activeTab="3" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -2154,7 +2154,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.5172413793103448E-2</c:v>
+                  <c:v>6.8965517241379309E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.9411764705882353E-2</c:v>
@@ -7562,7 +7562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -7665,7 +7665,7 @@
       </c>
       <c r="F3" s="49">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>0.1068714560805685</v>
+        <v>0.10759740889363566</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="22"/>
@@ -7695,7 +7695,7 @@
       </c>
       <c r="F4" s="50">
         <f ca="1">COUNTA(B2:B100)/$F$3</f>
-        <v>177.78367299193749</v>
+        <v>176.58417795899027</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22"/>
@@ -7725,7 +7725,7 @@
       </c>
       <c r="F5" s="51">
         <f ca="1">DATE(2022,7,17) + $F$4</f>
-        <v>44936.783672991936</v>
+        <v>44935.58417795899</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="22"/>
@@ -7858,14 +7858,14 @@
       </c>
       <c r="B11" s="28">
         <f>'Базы данных'!A3*100%/'Базы данных'!B3</f>
-        <v>5.5172413793103448E-2</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="C11" s="96" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="70">
         <f>SUM(B11:B14)/COUNTA(B11:B14)*100%</f>
-        <v>2.4398832728835671E-2</v>
+        <v>2.7847108590904637E-2</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="22"/>
@@ -8680,8 +8680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846B637B-365E-45A8-ACB1-45E326A5872F}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -8707,7 +8707,7 @@
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1">
       <c r="A3" s="7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="8">
         <v>145</v>

</xml_diff>

<commit_message>
update conspect update progress
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2710E68-22F8-489E-AC88-24A5C86FB7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61579C8D-194A-4086-966E-EA01AAB008D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="2325" windowWidth="35670" windowHeight="18330" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="1200" yWindow="2325" windowWidth="35670" windowHeight="18330" activeTab="3" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -2154,7 +2154,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.1103448275862069</c:v>
+                  <c:v>0.15862068965517243</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.9411764705882353E-2</c:v>
@@ -7562,7 +7562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -7665,7 +7665,7 @@
       </c>
       <c r="F3" s="49">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>0.10977526733283709</v>
+        <v>0.11231610217857213</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="22"/>
@@ -7695,7 +7695,7 @@
       </c>
       <c r="F4" s="50">
         <f ca="1">COUNTA(B2:B100)/$F$3</f>
-        <v>173.0808811641721</v>
+        <v>169.16541467751233</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22"/>
@@ -7725,7 +7725,7 @@
       </c>
       <c r="F5" s="51">
         <f ca="1">DATE(2022,7,17) + $F$4</f>
-        <v>44932.080881164169</v>
+        <v>44928.165414677511</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="22"/>
@@ -7858,14 +7858,14 @@
       </c>
       <c r="B11" s="28">
         <f>'Базы данных'!A3*100%/'Базы данных'!B3</f>
-        <v>0.1103448275862069</v>
+        <v>0.15862068965517243</v>
       </c>
       <c r="C11" s="96" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="70">
         <f>SUM(B11:B14)/COUNTA(B11:B14)*100%</f>
-        <v>3.819193617711153E-2</v>
+        <v>5.0260901694352919E-2</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="22"/>
@@ -8680,8 +8680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846B637B-365E-45A8-ACB1-45E326A5872F}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -8707,7 +8707,7 @@
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1">
       <c r="A3" s="7">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B3" s="8">
         <v>145</v>

</xml_diff>

<commit_message>
update binary search update conspect Algorytms update conspect
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E7FD30-A5D5-4728-9450-7BDBE215AF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066B28E9-F347-4856-8921-B5562063BA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="2790" windowWidth="35670" windowHeight="18330" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
@@ -1718,7 +1718,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3.9215686274509803E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7532,7 +7532,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="F3" s="49">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>0.11001859411419501</v>
+        <v>0.11188600774631452</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="22"/>
@@ -7664,7 +7664,7 @@
       </c>
       <c r="F4" s="50">
         <f ca="1">COUNTA(B2:B100)/$F$3</f>
-        <v>172.69808029248892</v>
+        <v>169.81569351441848</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22"/>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="F5" s="51">
         <f ca="1">DATE(2022,7,17) + $F$4</f>
-        <v>44931.698080292488</v>
+        <v>44928.815693514422</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="22"/>
@@ -7737,7 +7737,7 @@
       </c>
       <c r="D7" s="90">
         <f>SUM(B7:B9)/COUNTA(B7:B9)*100%</f>
-        <v>4.0160642570281129E-3</v>
+        <v>1.7087959681864714E-2</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="22"/>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="B9" s="30">
         <f>АиСД!A9*100%/АиСД!B9</f>
-        <v>0</v>
+        <v>3.9215686274509803E-2</v>
       </c>
       <c r="C9" s="89"/>
       <c r="D9" s="92"/>
@@ -8557,7 +8557,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -8627,7 +8627,8 @@
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1">
       <c r="A9" s="5">
-        <v>0</v>
+        <f>28-18</f>
+        <v>10</v>
       </c>
       <c r="B9" s="6">
         <v>255</v>

</xml_diff>

<commit_message>
update algorithms update progress
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066B28E9-F347-4856-8921-B5562063BA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76540575-A114-4601-8601-E28DDB34CC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="2790" windowWidth="35670" windowHeight="18330" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
@@ -1718,7 +1718,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9215686274509803E-2</c:v>
+                  <c:v>0.14117647058823529</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7532,7 +7532,7 @@
   <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="F3" s="49">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>0.11188600774631452</v>
+        <v>0.11674128318982524</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="22"/>
@@ -7664,7 +7664,7 @@
       </c>
       <c r="F4" s="50">
         <f ca="1">COUNTA(B2:B100)/$F$3</f>
-        <v>169.81569351441848</v>
+        <v>162.7530508561</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22"/>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="F5" s="51">
         <f ca="1">DATE(2022,7,17) + $F$4</f>
-        <v>44928.815693514422</v>
+        <v>44921.753050856103</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="22"/>
@@ -7737,7 +7737,7 @@
       </c>
       <c r="D7" s="90">
         <f>SUM(B7:B9)/COUNTA(B7:B9)*100%</f>
-        <v>1.7087959681864714E-2</v>
+        <v>5.1074887786439878E-2</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="22"/>
@@ -7785,7 +7785,7 @@
       </c>
       <c r="B9" s="30">
         <f>АиСД!A9*100%/АиСД!B9</f>
-        <v>3.9215686274509803E-2</v>
+        <v>0.14117647058823529</v>
       </c>
       <c r="C9" s="89"/>
       <c r="D9" s="92"/>
@@ -8557,7 +8557,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -8627,8 +8627,7 @@
     </row>
     <row r="9" spans="1:3" ht="16.5" thickBot="1">
       <c r="A9" s="5">
-        <f>28-18</f>
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B9" s="6">
         <v>255</v>

</xml_diff>

<commit_message>
update collection example code update progress
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9B8715-260E-4E4C-B98C-5D961E6173AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1029E73C-15B9-48D8-A971-5F13FAAC0B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="2790" windowWidth="35670" windowHeight="18330" activeTab="2" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="2220" yWindow="2790" windowWidth="35670" windowHeight="18330" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -1337,7 +1337,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2910052910052907E-2</c:v>
+                  <c:v>8.4656084656084651E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7531,8 +7531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -7597,7 +7597,7 @@
       </c>
       <c r="D2" s="84">
         <f>SUM(B2:B5)/COUNTA(B2:B5)*100%</f>
-        <v>0.21237139260395074</v>
+        <v>0.22030790054045868</v>
       </c>
       <c r="E2" s="47" t="s">
         <v>30</v>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="F3" s="49">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>0.106419364276473</v>
+        <v>0.1077996265263005</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="22"/>
@@ -7664,7 +7664,7 @@
       </c>
       <c r="F4" s="50">
         <f ca="1">COUNTA(B2:B100)/$F$3</f>
-        <v>178.5389353636694</v>
+        <v>176.25292973871723</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22"/>
@@ -7685,7 +7685,7 @@
       </c>
       <c r="B5" s="30">
         <f>Java!A12*100%/Java!B12</f>
-        <v>5.2910052910052907E-2</v>
+        <v>8.4656084656084651E-2</v>
       </c>
       <c r="C5" s="83"/>
       <c r="D5" s="86"/>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="F5" s="51">
         <f ca="1">DATE(2022,7,17) + $F$4</f>
-        <v>44937.538935363671</v>
+        <v>44935.252929738715</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="22"/>
@@ -8407,7 +8407,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -8465,7 +8465,8 @@
         <v>53</v>
       </c>
       <c r="E3" s="2">
-        <v>0</v>
+        <f>329-323</f>
+        <v>6</v>
       </c>
       <c r="F3" s="2">
         <f>361-323</f>
@@ -8533,7 +8534,7 @@
     <row r="12" spans="1:6" ht="16.5" thickBot="1">
       <c r="A12" s="17">
         <f>SUM(E2:E100)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B12" s="18">
         <f>SUM(F2:F100)</f>
@@ -8556,7 +8557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CEB77C-D1D9-44FA-A033-AAFB087AD5F9}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update conspect, progress, tasks
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1029E73C-15B9-48D8-A971-5F13FAAC0B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E225A14-45B8-4CB5-B4BD-B9FC3D434812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="2790" windowWidth="35670" windowHeight="18330" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
@@ -1337,7 +1337,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.4656084656084651E-2</c:v>
+                  <c:v>0.10582010582010581</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="F1" s="52">
         <f ca="1">TODAY() - DATE(2022,7,17)</f>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G1" s="53" t="s">
         <v>29</v>
@@ -7597,14 +7597,14 @@
       </c>
       <c r="D2" s="84">
         <f>SUM(B2:B5)/COUNTA(B2:B5)*100%</f>
-        <v>0.22030790054045868</v>
+        <v>0.22559890583146397</v>
       </c>
       <c r="E2" s="47" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="48">
         <f ca="1">$H$1-TODAY()</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="22"/>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="F3" s="49">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>0.1077996265263005</v>
+        <v>8.6226049354101109E-2</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="22"/>
@@ -7664,7 +7664,7 @@
       </c>
       <c r="F4" s="50">
         <f ca="1">COUNTA(B2:B100)/$F$3</f>
-        <v>176.25292973871723</v>
+        <v>220.35104405599577</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22"/>
@@ -7685,7 +7685,7 @@
       </c>
       <c r="B5" s="30">
         <f>Java!A12*100%/Java!B12</f>
-        <v>8.4656084656084651E-2</v>
+        <v>0.10582010582010581</v>
       </c>
       <c r="C5" s="83"/>
       <c r="D5" s="86"/>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="F5" s="51">
         <f ca="1">DATE(2022,7,17) + $F$4</f>
-        <v>44935.252929738715</v>
+        <v>44979.351044055998</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="22"/>
@@ -8407,7 +8407,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -8465,8 +8465,8 @@
         <v>53</v>
       </c>
       <c r="E3" s="2">
-        <f>329-323</f>
-        <v>6</v>
+        <f>333-323</f>
+        <v>10</v>
       </c>
       <c r="F3" s="2">
         <f>361-323</f>
@@ -8534,7 +8534,7 @@
     <row r="12" spans="1:6" ht="16.5" thickBot="1">
       <c r="A12" s="17">
         <f>SUM(E2:E100)</f>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" s="18">
         <f>SUM(F2:F100)</f>

</xml_diff>

<commit_message>
update progres, regexp conspect
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A710660F-DA09-4C5B-9EB4-B625CA297483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBA5183-41F3-4A23-AA3D-0C5178FEF340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="1590" windowWidth="35670" windowHeight="18330" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="1485" yWindow="1500" windowWidth="35670" windowHeight="18330" activeTab="1" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -1328,7 +1328,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.72093023255813948</c:v>
+                  <c:v>0.76744186046511631</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9.8901098901098897E-2</c:v>
@@ -7531,7 +7531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -7590,14 +7590,14 @@
       </c>
       <c r="B2" s="41">
         <f>Java!A3*100%/Java!B3</f>
-        <v>0.72093023255813948</v>
+        <v>0.76744186046511631</v>
       </c>
       <c r="C2" s="81" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="84">
         <f>SUM(B2:B5)/COUNTA(B2:B5)*100%</f>
-        <v>0.24464037254734927</v>
+        <v>0.25626827952409348</v>
       </c>
       <c r="E2" s="47" t="s">
         <v>30</v>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="F3" s="49">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>8.2667871410615865E-2</v>
+        <v>8.4077314680524234E-2</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="22"/>
@@ -7664,7 +7664,7 @@
       </c>
       <c r="F4" s="50">
         <f ca="1">COUNTA(B2:B100)/$F$3</f>
-        <v>229.83536016823217</v>
+        <v>225.98247900989614</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22"/>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="F5" s="51">
         <f ca="1">DATE(2022,7,17) + $F$4</f>
-        <v>44988.835360168232</v>
+        <v>44984.982479009894</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="22"/>
@@ -8406,8 +8406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D29483B-5B77-4D6C-8B76-A9E21F260E99}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -8456,7 +8456,7 @@
     </row>
     <row r="3" spans="1:6" ht="16.5" thickBot="1">
       <c r="A3" s="5">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="6">
         <v>43</v>

</xml_diff>

<commit_message>
update progres update sql conspect
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBA5183-41F3-4A23-AA3D-0C5178FEF340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4195513D-F084-4168-B079-795421FA0EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="1500" windowWidth="35670" windowHeight="18330" activeTab="1" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="1485" yWindow="1500" windowWidth="35670" windowHeight="18330" activeTab="3" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -2123,7 +2123,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.28275862068965518</c:v>
+                  <c:v>0.28965517241379313</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.9411764705882353E-2</c:v>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="F1" s="52">
         <f ca="1">TODAY() - DATE(2022,7,17)</f>
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G1" s="53" t="s">
         <v>29</v>
@@ -7604,7 +7604,7 @@
       </c>
       <c r="F2" s="48">
         <f ca="1">$H$1-TODAY()</f>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="22"/>
@@ -7634,7 +7634,7 @@
       </c>
       <c r="F3" s="49">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>8.4077314680524234E-2</v>
+        <v>7.7262442671706621E-2</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="22"/>
@@ -7664,7 +7664,7 @@
       </c>
       <c r="F4" s="50">
         <f ca="1">COUNTA(B2:B100)/$F$3</f>
-        <v>225.98247900989614</v>
+        <v>245.91508296899559</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22"/>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="F5" s="51">
         <f ca="1">DATE(2022,7,17) + $F$4</f>
-        <v>44984.982479009894</v>
+        <v>45004.915082968997</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="22"/>
@@ -7827,14 +7827,14 @@
       </c>
       <c r="B11" s="28">
         <f>'Базы данных'!A3*100%/'Базы данных'!B3</f>
-        <v>0.28275862068965518</v>
+        <v>0.28965517241379313</v>
       </c>
       <c r="C11" s="93" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="67">
         <f>SUM(B11:B14)/COUNTA(B11:B14)*100%</f>
-        <v>0.11159841475600391</v>
+        <v>0.11332255268703839</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="22"/>
@@ -8406,7 +8406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D29483B-5B77-4D6C-8B76-A9E21F260E99}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -8652,8 +8652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846B637B-365E-45A8-ACB1-45E326A5872F}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -8679,7 +8679,7 @@
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1">
       <c r="A3" s="7">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="8">
         <v>145</v>

</xml_diff>

<commit_message>
update conspect, update progress
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8710E83B-382E-4E80-98F7-3F774EB8188D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283D6FFA-9F9B-4018-8F48-60F6ED61E9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="1500" windowWidth="35670" windowHeight="18330" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="2505" yWindow="150" windowWidth="35670" windowHeight="18330" activeTab="3" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -957,6 +957,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="4" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1026,6 +1044,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="4" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1067,27 +1088,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="3" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2126,7 +2126,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.28965517241379313</c:v>
+                  <c:v>0.30344827586206896</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.9411764705882353E-2</c:v>
@@ -7396,7 +7396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -7420,18 +7420,18 @@
       <c r="B1" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="76"/>
+      <c r="D1" s="84"/>
       <c r="E1" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="101">
+      <c r="F1" s="64">
         <f ca="1">TODAY() - DATE(2022,7,17)</f>
-        <v>36</v>
-      </c>
-      <c r="G1" s="100" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="63" t="s">
         <v>29</v>
       </c>
       <c r="H1" s="51">
@@ -7457,14 +7457,14 @@
         <f>Java!A3*100%/Java!B3</f>
         <v>0.76744186046511631</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="80">
+      <c r="D2" s="88">
         <f>SUM(B2:B5)/COUNTA(B2:B5)*100%</f>
         <v>0.25626827952409348</v>
       </c>
-      <c r="E2" s="103" t="s">
+      <c r="E2" s="65" t="s">
         <v>54</v>
       </c>
       <c r="F2" s="48">
@@ -7491,14 +7491,14 @@
         <f>Java!A6*100%/Java!B6</f>
         <v>9.8901098901098897E-2</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="103" t="s">
+      <c r="C3" s="86"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="65" t="s">
         <v>55</v>
       </c>
       <c r="F3" s="49">
         <f ca="1">F1-F2</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="22"/>
@@ -7521,14 +7521,14 @@
         <f>Java!A9*100%/Java!B9</f>
         <v>0</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="107" t="s">
+      <c r="C4" s="86"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="108">
+      <c r="F4" s="70">
         <f ca="1">$H$1-TODAY()</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="22"/>
@@ -7551,8 +7551,8 @@
         <f>Java!A12*100%/Java!B12</f>
         <v>0.15873015873015872</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="82"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="90"/>
       <c r="G5" s="19"/>
       <c r="H5" s="22"/>
       <c r="I5" s="19"/>
@@ -7566,12 +7566,12 @@
       <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="E6" s="105" t="s">
+      <c r="E6" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="106">
+      <c r="F6" s="68">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>7.7262442671706621E-2</v>
+        <v>7.5547055125127396E-2</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="19"/>
@@ -7594,10 +7594,10 @@
         <f>АиСД!A3*100%/АиСД!B3</f>
         <v>1.2048192771084338E-2</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="102">
+      <c r="D7" s="94">
         <f>SUM(B7:B9)/COUNTA(B7:B9)*100%</f>
         <v>7.7218678636113078E-2</v>
       </c>
@@ -7606,7 +7606,7 @@
       </c>
       <c r="F7" s="49">
         <f ca="1">COUNTA(B2:B100)/$F$6</f>
-        <v>245.91508296899559</v>
+        <v>251.49888329241423</v>
       </c>
       <c r="G7" s="19"/>
       <c r="H7" s="19"/>
@@ -7629,14 +7629,14 @@
         <f>АиСД!A6*100%/АиСД!B6</f>
         <v>0</v>
       </c>
-      <c r="C8" s="84"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="104" t="s">
+      <c r="C8" s="92"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="66" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="50">
         <f ca="1">DATE(2022,7,17) + $F$7</f>
-        <v>45004.915082968997</v>
+        <v>45010.498883292414</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="19"/>
@@ -7659,8 +7659,8 @@
         <f>АиСД!A9*100%/АиСД!B9</f>
         <v>0.2196078431372549</v>
       </c>
-      <c r="C9" s="85"/>
-      <c r="D9" s="87"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="96"/>
       <c r="G9" s="19"/>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
@@ -7697,14 +7697,14 @@
       </c>
       <c r="B11" s="28">
         <f>'Базы данных'!A3*100%/'Базы данных'!B3</f>
-        <v>0.28965517241379313</v>
-      </c>
-      <c r="C11" s="88" t="s">
+        <v>0.30344827586206896</v>
+      </c>
+      <c r="C11" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="71">
         <f>SUM(B11:B14)/COUNTA(B11:B14)*100%</f>
-        <v>0.11332255268703839</v>
+        <v>0.11677082854910735</v>
       </c>
       <c r="E11" s="19"/>
       <c r="F11" s="22"/>
@@ -7729,8 +7729,8 @@
         <f>'Базы данных'!A6*100%/'Базы данных'!B6</f>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="C12" s="89"/>
-      <c r="D12" s="64"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="19"/>
       <c r="F12" s="22"/>
       <c r="G12" s="19"/>
@@ -7754,8 +7754,8 @@
         <f>'Базы данных'!A9*100%/'Базы данных'!B9</f>
         <v>0.12121212121212122</v>
       </c>
-      <c r="C13" s="89"/>
-      <c r="D13" s="64"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="19"/>
       <c r="F13" s="22"/>
       <c r="G13" s="19"/>
@@ -7779,8 +7779,8 @@
         <f>'Базы данных'!A12*100%/'Базы данных'!B12</f>
         <v>1.3011152416356878E-2</v>
       </c>
-      <c r="C14" s="90"/>
-      <c r="D14" s="65"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="19"/>
       <c r="F14" s="22"/>
       <c r="G14" s="19"/>
@@ -7820,10 +7820,10 @@
         <f>Сети!A3*100%/Сети!B3</f>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="C16" s="91" t="s">
+      <c r="C16" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="72">
+      <c r="D16" s="80">
         <f>SUM(B16:B18)/COUNTA(B16:B18)*100%</f>
         <v>2.3809523809523808E-2</v>
       </c>
@@ -7850,8 +7850,8 @@
         <f>Сети!A6*100%/Сети!B6</f>
         <v>0</v>
       </c>
-      <c r="C17" s="92"/>
-      <c r="D17" s="73"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="81"/>
       <c r="E17" s="19"/>
       <c r="F17" s="22"/>
       <c r="G17" s="19"/>
@@ -7875,8 +7875,8 @@
         <f>Сети!A9*100%/Сети!B9</f>
         <v>0</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="74"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="82"/>
       <c r="E18" s="19"/>
       <c r="F18" s="22"/>
       <c r="G18" s="19"/>
@@ -7960,10 +7960,10 @@
         <f>Spring!A3*100%/Spring!B3</f>
         <v>0</v>
       </c>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="69">
+      <c r="D22" s="77">
         <f>SUM(B22:B25)/COUNTA(B22:B25)*100%</f>
         <v>0</v>
       </c>
@@ -7990,8 +7990,8 @@
         <f>Spring!A6*100%/Spring!B6</f>
         <v>0</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="70"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="78"/>
       <c r="E23" s="19"/>
       <c r="F23" s="22"/>
       <c r="G23" s="19"/>
@@ -8015,8 +8015,8 @@
         <f>Spring!A9*100%/Spring!B9</f>
         <v>0</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="70"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="19"/>
       <c r="F24" s="22"/>
       <c r="G24" s="19"/>
@@ -8040,8 +8040,8 @@
         <f>Spring!A12*100%/Spring!B12</f>
         <v>0</v>
       </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="71"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="79"/>
       <c r="E25" s="19"/>
       <c r="F25" s="22"/>
       <c r="G25" s="19"/>
@@ -8292,10 +8292,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="104"/>
       <c r="D1" s="62" t="s">
         <v>52</v>
       </c>
@@ -8344,10 +8344,10 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="97"/>
+      <c r="B4" s="106"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
@@ -8366,10 +8366,10 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="97"/>
+      <c r="B7" s="106"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
@@ -8388,10 +8388,10 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="95"/>
+      <c r="B10" s="104"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
@@ -8439,10 +8439,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="104"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
@@ -8461,10 +8461,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="104"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
@@ -8483,10 +8483,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="104"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
@@ -8522,8 +8522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846B637B-365E-45A8-ACB1-45E326A5872F}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="15.75"/>
@@ -8534,10 +8534,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="104"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
@@ -8549,17 +8549,17 @@
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1">
       <c r="A3" s="7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="8">
         <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="104"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
@@ -8578,10 +8578,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="97"/>
+      <c r="B7" s="106"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
@@ -8600,10 +8600,10 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="103" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="95"/>
+      <c r="B10" s="104"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
@@ -8652,10 +8652,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="104"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
@@ -8674,10 +8674,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="104"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
@@ -8699,10 +8699,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="104"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
@@ -8746,10 +8746,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="95"/>
+      <c r="B1" s="104"/>
     </row>
     <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="3" t="s">
@@ -8791,10 +8791,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="99"/>
+      <c r="B1" s="108"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="9" t="s">
@@ -8816,10 +8816,10 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="95"/>
+      <c r="B4" s="104"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
@@ -8838,10 +8838,10 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="95"/>
+      <c r="B7" s="104"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
@@ -8860,10 +8860,10 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="95"/>
+      <c r="B10" s="104"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="15" t="s">

</xml_diff>

<commit_message>
add patterns to conspect
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shilaevvalentin/Documents/Java_Backend_Cource/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C393C9DE-C7DE-0144-8FF5-9D7656414C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB91601-CA1F-E14B-AEA3-D3DF91487A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19280" yWindow="2860" windowWidth="14320" windowHeight="17260" firstSheet="1" activeTab="6" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
     <sheet name="Java" sheetId="1" r:id="rId2"/>
-    <sheet name="АиСД" sheetId="2" r:id="rId3"/>
-    <sheet name="Базы данных" sheetId="3" r:id="rId4"/>
-    <sheet name="Сети" sheetId="4" r:id="rId5"/>
-    <sheet name="Git" sheetId="7" r:id="rId6"/>
-    <sheet name="Spring" sheetId="5" r:id="rId7"/>
+    <sheet name="ООП и Паттерны" sheetId="8" r:id="rId3"/>
+    <sheet name="АиСД" sheetId="2" r:id="rId4"/>
+    <sheet name="Базы данных" sheetId="3" r:id="rId5"/>
+    <sheet name="Сети" sheetId="4" r:id="rId6"/>
+    <sheet name="Git" sheetId="7" r:id="rId7"/>
+    <sheet name="Spring" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>Лекций просмотрено</t>
   </si>
@@ -209,6 +210,15 @@
   <si>
     <t>Дней с начала обучения прошло (полезные дни)</t>
   </si>
+  <si>
+    <t>Курс паттернов проектирования</t>
+  </si>
+  <si>
+    <t>Просмотрено</t>
+  </si>
+  <si>
+    <t>ООП и Паттерны проектирования</t>
+  </si>
 </sst>
 </file>
 
@@ -217,7 +227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +274,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -826,7 +843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1070,6 +1087,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7377,10 +7416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7388,7 +7427,7 @@
     <col min="1" max="1" width="52.796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.3984375" style="11" customWidth="1"/>
     <col min="3" max="3" width="24" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.3984375" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.19921875" style="12" customWidth="1"/>
     <col min="7" max="8" width="13.796875" style="1" customWidth="1"/>
@@ -7412,7 +7451,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">TODAY() - DATE(2022,7,17)</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>29</v>
@@ -7463,7 +7502,7 @@
       </c>
       <c r="F3" s="43">
         <f ca="1">F1-F2</f>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H3" s="12"/>
       <c r="P3" s="18"/>
@@ -7484,7 +7523,7 @@
       </c>
       <c r="F4" s="6">
         <f ca="1">$H$1-TODAY()</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="12"/>
       <c r="P4" s="18"/>
@@ -7509,7 +7548,7 @@
       </c>
       <c r="F6" s="61">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>5.1381861623574838E-2</v>
+        <v>5.1393270833823494E-2</v>
       </c>
       <c r="P6" s="18"/>
     </row>
@@ -7534,7 +7573,7 @@
       </c>
       <c r="F7" s="43">
         <f ca="1">COUNTA(B2:B100)/$F$6</f>
-        <v>369.78029599617486</v>
+        <v>389.1560057476899</v>
       </c>
       <c r="P7" s="18"/>
     </row>
@@ -7554,7 +7593,7 @@
       </c>
       <c r="F8" s="44">
         <f ca="1">DATE(2022,7,17) + $F$7</f>
-        <v>45128.780295996177</v>
+        <v>45148.156005747689</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -7740,6 +7779,15 @@
       </c>
       <c r="C25" s="68"/>
       <c r="D25" s="71"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27" s="11">
+        <f>'ООП и Паттерны'!A3*100%/'ООП и Паттерны'!B3</f>
+        <v>0.10344827586206896</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -7913,11 +7961,61 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31CADF6-A709-D946-8AEA-0CC28E48FB77}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView zoomScale="166" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.796875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="103" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="104"/>
+      <c r="C1" s="102"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="105" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="106" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="107">
+        <v>3</v>
+      </c>
+      <c r="B3" s="108">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="101"/>
+      <c r="B4" s="101"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CEB77C-D1D9-44FA-A033-AAFB087AD5F9}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.19921875" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8007,7 +8105,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846B637B-365E-45A8-ACB1-45E326A5872F}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -8125,7 +8223,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFCCA27-2B5A-43A0-8328-6BD008C1B7A2}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -8220,7 +8318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B851B2C-5898-47F3-9932-C07DFE0DFA15}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -8264,11 +8362,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCB3B14-49A5-43EF-AB59-F62EEDF89BCA}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add first CRUD application
</commit_message>
<xml_diff>
--- a/JavaBackend_progres.xlsx
+++ b/JavaBackend_progres.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4341F5-879D-4FE3-8DBA-D5F08A90F0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED05462-091A-4D4E-889B-AFB295C8BA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7230" yWindow="2865" windowWidth="29685" windowHeight="18240" activeTab="7" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
+    <workbookView xWindow="5325" yWindow="2055" windowWidth="29685" windowHeight="18240" xr2:uid="{81105D1A-FDE8-4E49-86A2-C9991C7F4C47}"/>
   </bookViews>
   <sheets>
     <sheet name="Анализ" sheetId="6" r:id="rId1"/>
@@ -3302,7 +3302,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.1368421052631579</c:v>
+                  <c:v>0.24210526315789474</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -7418,8 +7418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464BAAC1-1469-409E-BF4A-458009279AE4}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScaleSheetLayoutView="140" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7451,7 +7451,7 @@
       </c>
       <c r="F1" s="10">
         <f ca="1">TODAY() - DATE(2022,7,17)</f>
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="G1" s="57" t="s">
         <v>29</v>
@@ -7502,7 +7502,7 @@
       </c>
       <c r="F3" s="43">
         <f ca="1">F1-F2</f>
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="H3" s="12"/>
       <c r="P3" s="18"/>
@@ -7523,7 +7523,7 @@
       </c>
       <c r="F4" s="6">
         <f ca="1">$H$1-TODAY()</f>
-        <v>-14</v>
+        <v>-27</v>
       </c>
       <c r="H4" s="12"/>
       <c r="P4" s="18"/>
@@ -7548,7 +7548,7 @@
       </c>
       <c r="F6" s="61">
         <f ca="1">SUM($B$2:$B$100)/$F$1</f>
-        <v>4.4349765726190545E-2</v>
+        <v>3.8932710593480885E-2</v>
       </c>
       <c r="P6" s="18"/>
     </row>
@@ -7573,7 +7573,7 @@
       </c>
       <c r="F7" s="43">
         <f ca="1">COUNTA(B2:B100)/$F$6</f>
-        <v>450.96066850673566</v>
+        <v>513.70684689364816</v>
       </c>
       <c r="P7" s="18"/>
     </row>
@@ -7593,7 +7593,7 @@
       </c>
       <c r="F8" s="44">
         <f ca="1">DATE(2022,7,17) + $F$7</f>
-        <v>45209.960668506734</v>
+        <v>45272.706846893649</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7734,14 +7734,14 @@
       </c>
       <c r="B22" s="46">
         <f>Spring!A3*100%/Spring!B3</f>
-        <v>0.1368421052631579</v>
+        <v>0.24210526315789474</v>
       </c>
       <c r="C22" s="72" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="75">
         <f>SUM(B22:B25)/COUNTA(B22:B25)*100%</f>
-        <v>3.4210526315789476E-2</v>
+        <v>6.0526315789473685E-2</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8366,8 +8366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCB3B14-49A5-43EF-AB59-F62EEDF89BCA}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8393,7 +8393,7 @@
     </row>
     <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B3" s="8">
         <v>95</v>

</xml_diff>